<commit_message>
Importador de excel lee bien y sacado de main, falta que persista Consumos
</commit_message>
<xml_diff>
--- a/Codigo/ddsExcelv2.xlsx
+++ b/Codigo/ddsExcelv2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\Facultad\Diseño\2022-ma-ma-mama-grupo-05\Codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\Facultad\Diseño\9-11\2022-ma-ma-mama-grupo-05\Codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63217113-32F0-4E0F-A0C4-EF0B64A49877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD2C8B8-1E36-442D-BB61-08BE42738F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{542758CF-BFB6-4143-929E-4A55C3EB0BD9}"/>
+    <workbookView xWindow="5760" yWindow="2892" windowWidth="17280" windowHeight="8880" xr2:uid="{542758CF-BFB6-4143-929E-4A55C3EB0BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>COMBUSTION_FIJA</t>
   </si>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,10 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6D308F-B445-46B3-BAB7-E2C288C99CE4}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,36 +453,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44681</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
-        <v>44681</v>
+      <c r="E3" s="1">
+        <v>44682</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -491,16 +490,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <v>44682</v>
+      <c r="E4" s="1">
+        <v>44683</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -508,16 +507,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
-        <v>44683</v>
+      <c r="E5" s="1">
+        <v>44684</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -525,32 +524,15 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
-        <v>44684</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>800</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="E6" s="1">
         <v>44685</v>
       </c>
     </row>

</xml_diff>